<commit_message>
Update Heiankyo Alien - Plan.xlsx
Updated the leaderboards and added descriptions.
</commit_message>
<xml_diff>
--- a/Heiankyo Alien/Heiankyo Alien - Plan.xlsx
+++ b/Heiankyo Alien/Heiankyo Alien - Plan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17775" windowHeight="12135" firstSheet="10" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17775" windowHeight="12135" firstSheet="1" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="21" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4965" uniqueCount="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4967" uniqueCount="446">
   <si>
     <t>Description</t>
   </si>
@@ -1174,42 +1174,6 @@
     <t>New Game Overall Holes Dug</t>
   </si>
   <si>
-    <t>New Game Stage 12 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 1 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 2 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 3 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 4 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 5 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 6 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 7 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 8 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 9 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 10 Time</t>
-  </si>
-  <si>
-    <t>New Game Stage 11 Time</t>
-  </si>
-  <si>
     <t>New Game Overall Time</t>
   </si>
   <si>
@@ -1238,18 +1202,6 @@
   </si>
   <si>
     <t>Beat the new game market (stages 10-12)</t>
-  </si>
-  <si>
-    <t>New Game Market (Stages 10-12) Time</t>
-  </si>
-  <si>
-    <t>New Game Docks (Stages 7-9) Time</t>
-  </si>
-  <si>
-    <t>New Game Courtyard (Stages 4-6) Time</t>
-  </si>
-  <si>
-    <t>New Game Main Streets (Stages 1-3) Time</t>
   </si>
   <si>
     <t>0xTda06=1_0xNda19=0_0xMdaca=$Mode$S0x$5thPlace$&gt;=$5thValue$_0x$5thPlace$&lt;=9S0x$6thPlace$&gt;=$6thValue$_0x$6thPlace$&lt;=9</t>
@@ -1376,6 +1328,78 @@
   </si>
   <si>
     <t>N:0xNda19=0_P:0xMdaca=1_N:0xNda19=0_P:0xHdacc=0_</t>
+  </si>
+  <si>
+    <t>New Game Main Streets Time</t>
+  </si>
+  <si>
+    <t>New Game Courtyard Time</t>
+  </si>
+  <si>
+    <t>New Game Docks Time</t>
+  </si>
+  <si>
+    <t>New Game Market Time</t>
+  </si>
+  <si>
+    <t>Old Game Area 1 Time</t>
+  </si>
+  <si>
+    <t>Old Game Area 2 Time</t>
+  </si>
+  <si>
+    <t>Old Game Area 3 Time</t>
+  </si>
+  <si>
+    <t>Old Game Area 4 Time</t>
+  </si>
+  <si>
+    <t>Old Game Area 5 Time</t>
+  </si>
+  <si>
+    <t>The time it takes to complete all new game stages (stages 1-12)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the new game Main Streets (stages 1-3)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the new game Courtyard (stages 4-6)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the new game Docks (stages 7-9)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the new game Market (stages 10-12)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the old game Area 1 (stages 1-4)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the old game Area 2 (Stages 5-8)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the old game Area 3 (Stages 9-12)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the old game Area 4 (Stages 13-16)</t>
+  </si>
+  <si>
+    <t>The time it takes to complete the old game Area 5 (Stages 17-20)</t>
+  </si>
+  <si>
+    <t>The number of hole dug in the new game from the first stage until the player dies</t>
+  </si>
+  <si>
+    <t>The new game score from the first stage until the player dies</t>
+  </si>
+  <si>
+    <t>The number of holes dug in the old game from the first stage until the player dies</t>
+  </si>
+  <si>
+    <t>The old game score from the first stage until the player dies</t>
+  </si>
+  <si>
+    <t>The old game stage number from the first stage until the player dies</t>
   </si>
 </sst>
 </file>
@@ -10940,7 +10964,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -11275,397 +11299,397 @@
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="str">
         <f ca="1">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001001:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Start - New Game Main Streets (Stages 1-3) Time:Start - New Game Main Streets (Stages 1-3) Time::::Etron:0:::::00000</v>
+        <v>111001001:"The time it takes to complete the new game Main Streets (stages 1-3)":Start - New Game Main Streets Time:Start - New Game Main Streets Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="str">
         <f ca="1">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001002:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Main Streets (Stages 1-3) Time:Cancel - New Game Main Streets (Stages 1-3) Time::::Etron:0:::::00000</v>
+        <v>111001002:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Cancel - New Game Main Streets Time:Cancel - New Game Main Streets Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="str">
         <f ca="1">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001003:"0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=5_0xHdacb=6":Submit - New Game Main Streets (Stages 1-3) Time:Submit - New Game Main Streets (Stages 1-3) Time::::Etron:0:::::00000</v>
+        <v>111001003:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Submit - New Game Main Streets Time:Submit - New Game Main Streets Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="str">
         <f t="shared" ref="A60" ca="1" si="1">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001004:"0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=4_0xHdacb=5":Start - New Game Courtyard (Stages 4-6) Time:Start - New Game Courtyard (Stages 4-6) Time::::Etron:0:::::00000</v>
+        <v>111001004:"The time it takes to complete the new game Courtyard (stages 4-6)":Start - New Game Courtyard Time:Start - New Game Courtyard Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="str">
         <f t="shared" ref="A61" ca="1" si="2">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001005:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Courtyard (Stages 4-6) Time:Cancel - New Game Courtyard (Stages 4-6) Time::::Etron:0:::::00000</v>
+        <v>111001005:"0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=4_0xHdacb=5":Cancel - New Game Courtyard Time:Cancel - New Game Courtyard Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="str">
         <f t="shared" ref="A62" ca="1" si="3">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001006:"0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=5_0xHdacb=6":Submit - New Game Courtyard (Stages 4-6) Time:Submit - New Game Courtyard (Stages 4-6) Time::::Etron:0:::::00000</v>
+        <v>111001006:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Submit - New Game Courtyard Time:Submit - New Game Courtyard Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="str">
         <f t="shared" ref="A63" ca="1" si="4">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001007:"0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=4_0xHdacb=5":Start - New Game Docks (Stages 7-9) Time:Start - New Game Docks (Stages 7-9) Time::::Etron:0:::::00000</v>
+        <v>111001007:"The time it takes to complete the new game Docks (stages 7-9)":Start - New Game Docks Time:Start - New Game Docks Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="str">
         <f t="shared" ref="A64" ca="1" si="5">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001008:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Docks (Stages 7-9) Time:Cancel - New Game Docks (Stages 7-9) Time::::Etron:0:::::00000</v>
+        <v>111001008:"0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=4_0xHdacb=5":Cancel - New Game Docks Time:Cancel - New Game Docks Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="10" t="str">
         <f t="shared" ref="A65" ca="1" si="6">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001009:"0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=5_0xHdacb=6":Submit - New Game Docks (Stages 7-9) Time:Submit - New Game Docks (Stages 7-9) Time::::Etron:0:::::00000</v>
+        <v>111001009:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Submit - New Game Docks Time:Submit - New Game Docks Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="str">
         <f t="shared" ref="A66" ca="1" si="7">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001010:"0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=4_0xHdacb=5":Start - New Game Market (Stages 10-12) Time:Start - New Game Market (Stages 10-12) Time::::Etron:0:::::00000</v>
+        <v>111001010:"The time it takes to complete the new game Market (stages 10-12)":Start - New Game Market Time:Start - New Game Market Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="10" t="str">
         <f t="shared" ref="A67" ca="1" si="8">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001011:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Market (Stages 10-12) Time:Cancel - New Game Market (Stages 10-12) Time::::Etron:0:::::00000</v>
+        <v>111001011:"0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=4_0xHdacb=5":Cancel - New Game Market Time:Cancel - New Game Market Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="10" t="str">
         <f t="shared" ref="A68" ca="1" si="9">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001012:"0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6":Submit - New Game Market (Stages 10-12) Time:Submit - New Game Market (Stages 10-12) Time::::Etron:0:::::00000</v>
+        <v>111001012:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Submit - New Game Market Time:Submit - New Game Market Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="10" t="str">
         <f t="shared" ref="A69" ca="1" si="10">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001013:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 1 Time:Start - New Game Stage 1 Time::::Etron:0:::::00000</v>
+        <v>111001013:"The time it takes to complete all new game stages (stages 1-12)":Start - New Game Overall Time:Start - New Game Overall Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="10" t="str">
         <f t="shared" ref="A70" ca="1" si="11">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001014:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 1 Time:Cancel - New Game Stage 1 Time::::Etron:0:::::00000</v>
+        <v>111001014:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Cancel - New Game Overall Time:Cancel - New Game Overall Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="10" t="str">
         <f t="shared" ref="A71" ca="1" si="12">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001015:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 1 Time:Submit - New Game Stage 1 Time::::Etron:0:::::00000</v>
+        <v>111001015:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Submit - New Game Overall Time:Submit - New Game Overall Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="10" t="str">
         <f t="shared" ref="A72" ca="1" si="13">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001016:"0xNda19=0_0xMdaca=1_0xHdacd=1_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 2 Time:Start - New Game Stage 2 Time::::Etron:0:::::00000</v>
+        <v>111001016:"The new game score from the first stage until the player dies":Start - New Game Overall High Score:Start - New Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="10" t="str">
         <f t="shared" ref="A73" ca="1" si="14">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001017:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 2 Time:Cancel - New Game Stage 2 Time::::Etron:0:::::00000</v>
+        <v>111001017:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Cancel - New Game Overall High Score:Cancel - New Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="10" t="str">
         <f t="shared" ref="A74" ca="1" si="15">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001018:"0xNda19=0_0xMdaca=1_0xHdacd=1_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 2 Time:Submit - New Game Stage 2 Time::::Etron:0:::::00000</v>
+        <v>111001018:"":Submit - New Game Overall High Score:Submit - New Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="10" t="str">
         <f t="shared" ref="A75" ca="1" si="16">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001019:"0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 3 Time:Start - New Game Stage 3 Time::::Etron:0:::::00000</v>
+        <v>111001019:"The number of hole dug in the new game from the first stage until the player dies":Start - New Game Overall Holes Dug:Start - New Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="10" t="str">
         <f t="shared" ref="A76" ca="1" si="17">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001020:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 3 Time:Cancel - New Game Stage 3 Time::::Etron:0:::::00000</v>
+        <v>111001020:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Cancel - New Game Overall Holes Dug:Cancel - New Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="10" t="str">
         <f t="shared" ref="A77" ca="1" si="18">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001021:"0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 3 Time:Submit - New Game Stage 3 Time::::Etron:0:::::00000</v>
+        <v>111001021:"":Submit - New Game Overall Holes Dug:Submit - New Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="str">
         <f t="shared" ref="A78" ca="1" si="19">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001022:"0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 4 Time:Start - New Game Stage 4 Time::::Etron:0:::::00000</v>
+        <v>111001022:"The time it takes to complete the old game Area 1 (stages 1-4)":Start - Old Game Area 1 Time:Start - Old Game Area 1 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="str">
         <f t="shared" ref="A79" ca="1" si="20">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001023:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 4 Time:Cancel - New Game Stage 4 Time::::Etron:0:::::00000</v>
+        <v>111001023:"":Cancel - Old Game Area 1 Time:Cancel - Old Game Area 1 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="10" t="str">
         <f t="shared" ref="A80" ca="1" si="21">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001024:"0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 4 Time:Submit - New Game Stage 4 Time::::Etron:0:::::00000</v>
+        <v>111001024:"":Submit - Old Game Area 1 Time:Submit - Old Game Area 1 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="10" t="str">
         <f t="shared" ref="A81" ca="1" si="22">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001025:"0xNda19=0_0xMdaca=1_0xHdacd=4_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 5 Time:Start - New Game Stage 5 Time::::Etron:0:::::00000</v>
+        <v>111001025:"The time it takes to complete the old game Area 2 (Stages 5-8)":Start - Old Game Area 2 Time:Start - Old Game Area 2 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="10" t="str">
         <f t="shared" ref="A82" ca="1" si="23">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001026:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 5 Time:Cancel - New Game Stage 5 Time::::Etron:0:::::00000</v>
+        <v>111001026:"":Cancel - Old Game Area 2 Time:Cancel - Old Game Area 2 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="10" t="str">
         <f t="shared" ref="A83" ca="1" si="24">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001027:"0xNda19=0_0xMdaca=1_0xHdacd=4_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 5 Time:Submit - New Game Stage 5 Time::::Etron:0:::::00000</v>
+        <v>111001027:"":Submit - Old Game Area 2 Time:Submit - Old Game Area 2 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="10" t="str">
         <f t="shared" ref="A84" ca="1" si="25">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001028:"0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 6 Time:Start - New Game Stage 6 Time::::Etron:0:::::00000</v>
+        <v>111001028:"The time it takes to complete the old game Area 3 (Stages 9-12)":Start - Old Game Area 3 Time:Start - Old Game Area 3 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="10" t="str">
         <f t="shared" ref="A85" ca="1" si="26">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001029:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 6 Time:Cancel - New Game Stage 6 Time::::Etron:0:::::00000</v>
+        <v>111001029:"":Cancel - Old Game Area 3 Time:Cancel - Old Game Area 3 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="10" t="str">
         <f t="shared" ref="A86" ca="1" si="27">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001030:"0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 6 Time:Submit - New Game Stage 6 Time::::Etron:0:::::00000</v>
+        <v>111001030:"":Submit - Old Game Area 3 Time:Submit - Old Game Area 3 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="10" t="str">
         <f t="shared" ref="A87" ca="1" si="28">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001031:"0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 7 Time:Start - New Game Stage 7 Time::::Etron:0:::::00000</v>
+        <v>111001031:"The time it takes to complete the old game Area 4 (Stages 13-16)":Start - Old Game Area 4 Time:Start - Old Game Area 4 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="10" t="str">
         <f t="shared" ref="A88" ca="1" si="29">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001032:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 7 Time:Cancel - New Game Stage 7 Time::::Etron:0:::::00000</v>
+        <v>111001032:"":Cancel - Old Game Area 4 Time:Cancel - Old Game Area 4 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="10" t="str">
         <f t="shared" ref="A89" ca="1" si="30">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001033:"0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 7 Time:Submit - New Game Stage 7 Time::::Etron:0:::::00000</v>
+        <v>111001033:"":Submit - Old Game Area 4 Time:Submit - Old Game Area 4 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="10" t="str">
         <f t="shared" ref="A90" ca="1" si="31">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001034:"0xNda19=0_0xMdaca=1_0xHdacd=7_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 8 Time:Start - New Game Stage 8 Time::::Etron:0:::::00000</v>
+        <v>111001034:"The time it takes to complete the old game Area 5 (Stages 17-20)":Start - Old Game Area 5 Time:Start - Old Game Area 5 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="10" t="str">
         <f t="shared" ref="A91" ca="1" si="32">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001035:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 8 Time:Cancel - New Game Stage 8 Time::::Etron:0:::::00000</v>
+        <v>111001035:"":Cancel - Old Game Area 5 Time:Cancel - Old Game Area 5 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="10" t="str">
         <f t="shared" ref="A92" ca="1" si="33">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001036:"0xNda19=0_0xMdaca=1_0xHdacd=7_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 8 Time:Submit - New Game Stage 8 Time::::Etron:0:::::00000</v>
+        <v>111001036:"":Submit - Old Game Area 5 Time:Submit - Old Game Area 5 Time::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="10" t="str">
         <f t="shared" ref="A93" ca="1" si="34">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001037:"0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 9 Time:Start - New Game Stage 9 Time::::Etron:0:::::00000</v>
+        <v>111001037:"The old game stage number from the first stage until the player dies":Start - Old Game Overall Highest Stage:Start - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="10" t="str">
         <f t="shared" ref="A94" ca="1" si="35">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001038:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 9 Time:Cancel - New Game Stage 9 Time::::Etron:0:::::00000</v>
+        <v>111001038:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Cancel - Old Game Overall Highest Stage:Cancel - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="10" t="str">
         <f t="shared" ref="A95" ca="1" si="36">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001039:"0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 9 Time:Submit - New Game Stage 9 Time::::Etron:0:::::00000</v>
+        <v>111001039:"":Submit - Old Game Overall Highest Stage:Submit - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="10" t="str">
         <f t="shared" ref="A96" ca="1" si="37">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001040:"0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 10 Time:Start - New Game Stage 10 Time::::Etron:0:::::00000</v>
+        <v>111001040:"The old game score from the first stage until the player dies":Start - Old Game Overall High Score:Start - Old Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="10" t="str">
         <f t="shared" ref="A97" ca="1" si="38">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001041:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 10 Time:Cancel - New Game Stage 10 Time::::Etron:0:::::00000</v>
+        <v>111001041:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Cancel - Old Game Overall High Score:Cancel - Old Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="10" t="str">
         <f t="shared" ref="A98" ca="1" si="39">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001042:"0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 10 Time:Submit - New Game Stage 10 Time::::Etron:0:::::00000</v>
+        <v>111001042:"":Submit - Old Game Overall High Score:Submit - Old Game Overall High Score::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="10" t="str">
         <f t="shared" ref="A99" ca="1" si="40">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001043:"0xNda19=0_0xMdaca=1_0xHdacd=10_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 11 Time:Start - New Game Stage 11 Time::::Etron:0:::::00000</v>
+        <v>111001043:"The number of holes dug in the old game from the first stage until the player dies":Start - Old Game Overall Holes Dug:Start - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="10" t="str">
         <f t="shared" ref="A100" ca="1" si="41">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001044:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 11 Time:Cancel - New Game Stage 11 Time::::Etron:0:::::00000</v>
+        <v>111001044:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Cancel - Old Game Overall Holes Dug:Cancel - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="str">
         <f t="shared" ref="A101" ca="1" si="42">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001045:"0xNda19=0_0xMdaca=1_0xHdacd=10_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 11 Time:Submit - New Game Stage 11 Time::::Etron:0:::::00000</v>
+        <v>111001045:"":Submit - Old Game Overall Holes Dug:Submit - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="str">
         <f t="shared" ref="A102" ca="1" si="43">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001046:"0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=4_0xHdacb=5":Start - New Game Stage 12 Time:Start - New Game Stage 12 Time::::Etron:0:::::00000</v>
+        <v>111001046:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="10" t="str">
         <f t="shared" ref="A103" ca="1" si="44">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001047:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Stage 12 Time:Cancel - New Game Stage 12 Time::::Etron:0:::::00000</v>
+        <v>111001047:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="10" t="str">
         <f t="shared" ref="A104" ca="1" si="45">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001048:"0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6":Submit - New Game Stage 12 Time:Submit - New Game Stage 12 Time::::Etron:0:::::00000</v>
+        <v>111001048:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="10" t="str">
         <f t="shared" ref="A105" ca="1" si="46">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001049:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Start - New Game Overall Time:Start - New Game Overall Time::::Etron:0:::::00000</v>
+        <v>111001049:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="10" t="str">
         <f t="shared" ref="A106" ca="1" si="47">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001050:"0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9":Cancel - New Game Overall Time:Cancel - New Game Overall Time::::Etron:0:::::00000</v>
+        <v>111001050:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="10" t="str">
         <f t="shared" ref="A107" ca="1" si="48">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001051:"0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6":Submit - New Game Overall Time:Submit - New Game Overall Time::::Etron:0:::::00000</v>
+        <v>111001051:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="10" t="str">
         <f t="shared" ref="A108" ca="1" si="49">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001052:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Start - New Game Overall High Score:Start - New Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001052:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="10" t="str">
         <f t="shared" ref="A109" ca="1" si="50">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001053:"":Cancel - New Game Overall High Score:Cancel - New Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001053:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="10" t="str">
         <f t="shared" ref="A110" ca="1" si="51">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001054:"0xNda19=0_0xMdaca=1S0xHdacd=11_d0xHdacb=5_0xHdacb=6Sd0xHdacb=12_0xHdacb=9":Submit - New Game Overall High Score:Submit - New Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001054:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="10" t="str">
         <f t="shared" ref="A111" ca="1" si="52">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001055:"0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5":Start - New Game Overall Holes Dug:Start - New Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001055:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="10" t="str">
         <f t="shared" ref="A112" ca="1" si="53">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001056:"":Cancel - New Game Overall Holes Dug:Cancel - New Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001056:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="10" t="str">
         <f t="shared" ref="A113" ca="1" si="54">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001057:"0xNda19=0_0xMdaca=1S0xHdacd=11_d0xHdacb=5_0xHdacb=6Sd0xHdacb=12_0xHdacb=9":Submit - New Game Overall Holes Dug:Submit - New Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001057:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="10" t="str">
         <f t="shared" ref="A114" ca="1" si="55">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001058:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Start - Old Game Overall Highest Stage:Start - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
+        <v>111001058:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="10" t="str">
         <f t="shared" ref="A115" ca="1" si="56">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001059:"":Cancel - Old Game Overall Highest Stage:Cancel - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
+        <v>111001059:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="10" t="str">
         <f t="shared" ref="A116" ca="1" si="57">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001060:"0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0":Submit - Old Game Overall Highest Stage:Submit - Old Game Overall Highest Stage::::Etron:0:::::00000</v>
+        <v>111001060:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="10" t="str">
         <f t="shared" ref="A117" ca="1" si="58">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001061:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Start - Old Game Overall High Score:Start - Old Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001061:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="10" t="str">
         <f t="shared" ref="A118" ca="1" si="59">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001062:"":Cancel - Old Game Overall High Score:Cancel - Old Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001062:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="10" t="str">
         <f t="shared" ref="A119" ca="1" si="60">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001063:"0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0":Submit - Old Game Overall High Score:Submit - Old Game Overall High Score::::Etron:0:::::00000</v>
+        <v>111001063:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="10" t="str">
         <f t="shared" ref="A120" ca="1" si="61">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!B"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Start - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001064:"0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8":Start - Old Game Overall Holes Dug:Start - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001064:"":Start - :Start - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="10" t="str">
         <f t="shared" ref="A121" ca="1" si="62">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!C"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Cancel - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001065:"":Cancel - Old Game Overall Holes Dug:Cancel - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001065:"":Cancel - :Cancel - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="10" t="str">
         <f t="shared" ref="A122" ca="1" si="63">"111001"&amp;TEXT(ROW()-56,"000")&amp;":"&amp;CHAR(34)&amp;INDIRECT("Leaderboards!D"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;CHAR(34)&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;":Submit - "&amp;INDIRECT("Leaderboards!A"&amp;(2+ROUNDDOWN((ROW()-57)/3,0)))&amp;"::::Etron:0:::::00000"</f>
-        <v>111001066:"0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0":Submit - Old Game Overall Holes Dug:Submit - Old Game Overall Holes Dug::::Etron:0:::::00000</v>
+        <v>111001066:"":Submit - :Submit - ::::Etron:0:::::00000</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
@@ -11935,7 +11959,7 @@
         <v>161</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -11944,19 +11968,19 @@
         <v>162</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>77</v>
@@ -11967,10 +11991,10 @@
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D5" s="10">
         <f>HEX2DEC(C5)</f>
@@ -11993,10 +12017,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D6" s="10">
         <f t="shared" ref="D6:D8" si="0">HEX2DEC(C6)</f>
@@ -12019,10 +12043,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D7" s="10">
         <f t="shared" si="0"/>
@@ -12045,10 +12069,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D8" s="10">
         <f t="shared" si="0"/>
@@ -12071,10 +12095,10 @@
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D9" s="10">
         <f>HEX2DEC(C9)</f>
@@ -12097,10 +12121,10 @@
         <v>1</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D10" s="10">
         <f t="shared" ref="D10:F21" si="3">HEX2DEC(C10)</f>
@@ -12123,10 +12147,10 @@
         <v>1</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D11" s="10">
         <f t="shared" si="3"/>
@@ -12149,10 +12173,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D12" s="10">
         <f t="shared" si="3"/>
@@ -12175,10 +12199,10 @@
         <v>1</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D13" s="10">
         <f t="shared" si="3"/>
@@ -12201,10 +12225,10 @@
         <v>1</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D14" s="10">
         <f t="shared" si="3"/>
@@ -12227,10 +12251,10 @@
         <v>1</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D15" s="10">
         <f t="shared" si="3"/>
@@ -12253,10 +12277,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D16" s="10">
         <f t="shared" si="3"/>
@@ -12279,10 +12303,10 @@
         <v>1</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D17" s="10">
         <f t="shared" si="3"/>
@@ -12305,10 +12329,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D18" s="10">
         <f t="shared" si="3"/>
@@ -12331,10 +12355,10 @@
         <v>1</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D19" s="10">
         <f t="shared" si="3"/>
@@ -12357,10 +12381,10 @@
         <v>1</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D20" s="10">
         <f t="shared" si="3"/>
@@ -12383,10 +12407,10 @@
         <v>1</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="D21" s="10">
         <f t="shared" si="3"/>
@@ -12409,7 +12433,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="C22" s="23">
         <v>11</v>
@@ -12435,7 +12459,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="C23" s="23">
         <v>11</v>
@@ -12461,7 +12485,7 @@
         <v>0</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="C24" s="23">
         <v>11</v>
@@ -12507,23 +12531,23 @@
         <v>161</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -12534,37 +12558,37 @@
         <v>148</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>164</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="L4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="M4" s="10" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="N4" s="10" t="s">
         <v>77</v>
@@ -12582,7 +12606,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F5" s="23">
         <v>5</v>
@@ -12617,7 +12641,7 @@
         <v>5</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F6" s="23">
         <v>5</v>
@@ -12652,7 +12676,7 @@
         <v>8</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F7" s="23">
         <v>5</v>
@@ -12687,7 +12711,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F8" s="23">
         <v>5</v>
@@ -12722,7 +12746,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F9" s="23">
         <v>5</v>
@@ -12757,7 +12781,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F10" s="23">
         <v>5</v>
@@ -12792,7 +12816,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F11" s="23">
         <v>5</v>
@@ -12827,7 +12851,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F12" s="23">
         <v>5</v>
@@ -12862,7 +12886,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F13" s="23">
         <v>5</v>
@@ -12897,7 +12921,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F14" s="23">
         <v>5</v>
@@ -12932,7 +12956,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F15" s="23">
         <v>5</v>
@@ -12967,7 +12991,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F16" s="23">
         <v>5</v>
@@ -13002,7 +13026,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F17" s="23">
         <v>5</v>
@@ -13037,7 +13061,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F18" s="23">
         <v>5</v>
@@ -13072,7 +13096,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F19" s="23">
         <v>5</v>
@@ -13107,7 +13131,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F20" s="23">
         <v>5</v>
@@ -13142,7 +13166,7 @@
         <v>11</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F21" s="23">
         <v>5</v>
@@ -13177,7 +13201,7 @@
         <v>11</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F22" s="23">
         <v>5</v>
@@ -13194,7 +13218,7 @@
         <v>6</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="K22" s="10">
         <f t="shared" ref="K22:K23" si="8">HEX2DEC(J22)</f>
@@ -13224,7 +13248,7 @@
         <v>11</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F23" s="23">
         <v>5</v>
@@ -13241,7 +13265,7 @@
         <v>6</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="K23" s="10">
         <f t="shared" si="8"/>
@@ -13433,13 +13457,13 @@
         <v>158</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D4" t="s">
         <v>163</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="F4" t="s">
         <v>164</v>
@@ -13697,7 +13721,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="F14" s="10">
         <f t="shared" si="0"/>
@@ -13716,14 +13740,14 @@
         <v>83</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="D15" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="F15" s="10">
         <f t="shared" si="0"/>
@@ -13742,14 +13766,14 @@
         <v>83</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="D16" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
       <c r="F16" s="10">
         <f t="shared" si="0"/>
@@ -14304,7 +14328,7 @@
         <v>179</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -15032,7 +15056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CM68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
@@ -39268,10 +39292,10 @@
         <v>75</v>
       </c>
       <c r="X4" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y4" s="14" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -40180,9 +40204,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:A76"/>
+  <dimension ref="A1:A94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A54" workbookViewId="0">
+      <selection activeCell="A92" sqref="A85:A92"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -40641,6 +40667,108 @@
       <c r="A76" t="str">
         <f>"Total Set ("&amp;COUNTA(Achievements!A:A)-1 &amp;" Achievements - "&amp;SUM(Achievements!F:F)&amp;" Points)"</f>
         <v>Total Set (54 Achievements - 365 Points)</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="10" t="str">
+        <f ca="1">"[b]"&amp;INDIRECT("Leaderboards!A"&amp;(ROW()-76))&amp;"[/b] - "&amp;INDIRECT("Leaderboards!B"&amp;(ROW()-76))</f>
+        <v>[b]New Game Main Streets Time[/b] - The time it takes to complete the new game Main Streets (stages 1-3)</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="10" t="str">
+        <f t="shared" ref="A79:A94" ca="1" si="3">"[b]"&amp;INDIRECT("Leaderboards!A"&amp;(ROW()-76))&amp;"[/b] - "&amp;INDIRECT("Leaderboards!B"&amp;(ROW()-76))</f>
+        <v>[b]New Game Courtyard Time[/b] - The time it takes to complete the new game Courtyard (stages 4-6)</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]New Game Docks Time[/b] - The time it takes to complete the new game Docks (stages 7-9)</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]New Game Market Time[/b] - The time it takes to complete the new game Market (stages 10-12)</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]New Game Overall Time[/b] - The time it takes to complete all new game stages (stages 1-12)</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]New Game Overall High Score[/b] - The new game score from the first stage until the player dies</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]New Game Overall Holes Dug[/b] - The number of hole dug in the new game from the first stage until the player dies</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Area 1 Time[/b] - The time it takes to complete the old game Area 1 (stages 1-4)</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Area 2 Time[/b] - The time it takes to complete the old game Area 2 (Stages 5-8)</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Area 3 Time[/b] - The time it takes to complete the old game Area 3 (Stages 9-12)</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Area 4 Time[/b] - The time it takes to complete the old game Area 4 (Stages 13-16)</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Area 5 Time[/b] - The time it takes to complete the old game Area 5 (Stages 17-20)</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Overall Highest Stage[/b] - The old game stage number from the first stage until the player dies</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v>[b]Old Game Overall High Score[/b] - The old game score from the first stage until the player dies</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="10" t="str">
+        <f ca="1">"[b]"&amp;INDIRECT("Leaderboards!A"&amp;(ROW()-76))&amp;"[/b] - "&amp;INDIRECT("Leaderboards!B"&amp;(ROW()-76))</f>
+        <v>[b]Old Game Overall Holes Dug[/b] - The number of holes dug in the old game from the first stage until the player dies</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v xml:space="preserve">[b][/b] - </v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="10" t="str">
+        <f t="shared" ca="1" si="3"/>
+        <v xml:space="preserve">[b][/b] - </v>
       </c>
     </row>
   </sheetData>
@@ -40994,10 +41122,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -41571,7 +41699,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -42559,10 +42687,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -43025,7 +43153,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -44139,10 +44267,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -44638,7 +44766,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -45734,10 +45862,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -46191,7 +46319,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -47235,10 +47363,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -47716,7 +47844,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -48764,10 +48892,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -49227,7 +49355,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -50357,10 +50485,10 @@
         <v>75</v>
       </c>
       <c r="X6" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y6" s="14" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -50856,7 +50984,7 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="P23" s="14" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="V23" s="14" t="str">
         <f>$Y$6&amp;$V$22</f>
@@ -52023,8 +52151,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:K89"/>
   <sheetViews>
-    <sheetView topLeftCell="F28" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52099,7 +52227,7 @@
         <v>3</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>388</v>
+        <v>376</v>
       </c>
       <c r="H2" s="1"/>
       <c r="J2" s="24">
@@ -52131,7 +52259,7 @@
         <v>5</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="6"/>
@@ -52164,7 +52292,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="H4" s="1"/>
       <c r="J4" s="24">
@@ -52196,7 +52324,7 @@
         <v>25</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>391</v>
+        <v>379</v>
       </c>
       <c r="H5" s="1"/>
       <c r="J5" s="24">
@@ -52556,7 +52684,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="H16" s="1"/>
       <c r="J16" s="24">
@@ -52587,7 +52715,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="H17" s="1"/>
       <c r="J17" s="24">
@@ -52649,7 +52777,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="H19" s="1"/>
       <c r="J19" s="24">
@@ -52713,7 +52841,7 @@
         <v>5</v>
       </c>
       <c r="G21" s="7" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="H21" s="1"/>
       <c r="J21" s="24">
@@ -52907,7 +53035,7 @@
         <v>5</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>421</v>
+        <v>405</v>
       </c>
       <c r="H27" s="1"/>
       <c r="J27" s="24">
@@ -52939,7 +53067,7 @@
         <v>5</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>422</v>
+        <v>406</v>
       </c>
       <c r="H28" s="1"/>
       <c r="J28" s="24">
@@ -52971,7 +53099,7 @@
         <v>10</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>423</v>
+        <v>407</v>
       </c>
       <c r="H29" s="1"/>
       <c r="J29" s="24">
@@ -53003,7 +53131,7 @@
         <v>25</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="H30" s="1"/>
       <c r="J30" s="24">
@@ -53035,7 +53163,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="H31" s="1"/>
       <c r="I31" s="10"/>
@@ -53068,7 +53196,7 @@
         <v>5</v>
       </c>
       <c r="G32" s="7" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="H32" s="1"/>
       <c r="J32" s="19">
@@ -53100,7 +53228,7 @@
         <v>5</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="H33" s="1"/>
       <c r="J33" s="19">
@@ -53132,7 +53260,7 @@
         <v>10</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="H34" s="1"/>
       <c r="I34" s="6"/>
@@ -53165,7 +53293,7 @@
         <v>25</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>420</v>
+        <v>404</v>
       </c>
       <c r="H35" s="1"/>
       <c r="J35" s="19">
@@ -53526,7 +53654,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="H46" s="1"/>
       <c r="I46" s="10"/>
@@ -53559,7 +53687,7 @@
         <v>3</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="H47" s="1"/>
       <c r="J47" s="19">
@@ -53623,7 +53751,7 @@
         <v>10</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="H49" s="1"/>
       <c r="J49" s="19">
@@ -54336,10 +54464,10 @@
         <v>75</v>
       </c>
       <c r="X4" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y4" s="14" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -55585,10 +55713,10 @@
         <v>75</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -56736,10 +56864,10 @@
         <v>75</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -57889,10 +58017,10 @@
         <v>75</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -58849,10 +58977,10 @@
         <v>75</v>
       </c>
       <c r="X5" s="14" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="Y5" s="14" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -61148,461 +61276,310 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="80.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
+    <col min="2" max="2" width="75.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
-        <v>383</v>
+        <v>371</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>384</v>
+        <v>0</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>385</v>
+        <v>372</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>386</v>
+        <v>373</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+        <v>374</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>395</v>
-      </c>
-      <c r="B2" s="10" t="str">
+        <v>422</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" s="10" t="str">
         <f>Start!J5</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C2" s="10" t="str">
+      <c r="D2" s="10" t="str">
         <f>Cancel!G5</f>
         <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="D2" s="10" t="str">
+      <c r="E2" s="10" t="str">
         <f>Submit!N5</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=5_0xHdacb=6</v>
       </c>
-      <c r="E2" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F2" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>394</v>
-      </c>
-      <c r="B3" s="10" t="str">
+        <v>423</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>433</v>
+      </c>
+      <c r="C3" s="10" t="str">
         <f>Start!J6</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C3" s="10" t="str">
+      <c r="D3" s="10" t="str">
         <f>Cancel!G6</f>
         <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="D3" s="10" t="str">
+      <c r="E3" s="10" t="str">
         <f>Submit!N6</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=5_0xHdacb=6</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>393</v>
-      </c>
-      <c r="B4" s="10" t="str">
+        <v>424</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="C4" s="10" t="str">
         <f>Start!J7</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="D4" s="10" t="str">
         <f>Cancel!G7</f>
         <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="E4" s="10" t="str">
         <f>Submit!N7</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=5_0xHdacb=6</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F4" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>392</v>
-      </c>
-      <c r="B5" s="10" t="str">
+        <v>425</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="C5" s="10" t="str">
         <f>Start!J8</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C5" s="10" t="str">
+      <c r="D5" s="10" t="str">
         <f>Cancel!G8</f>
         <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="D5" s="10" t="str">
+      <c r="E5" s="10" t="str">
         <f>Submit!N8</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F5" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="B6" s="10" t="str">
-        <f>Start!J9</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5</v>
+        <v>370</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>431</v>
       </c>
       <c r="C6" s="10" t="str">
-        <f>Cancel!G9</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D6" s="10" t="str">
-        <f>Submit!N9</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="B7" s="10" t="str">
-        <f>Start!J10</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=1_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C7" s="10" t="str">
-        <f>Cancel!G10</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D7" s="10" t="str">
-        <f>Submit!N10</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=1_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="B8" s="10" t="str">
-        <f>Start!J11</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C8" s="10" t="str">
-        <f>Cancel!G11</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D8" s="10" t="str">
-        <f>Submit!N11</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=2_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="B9" s="10" t="str">
-        <f>Start!J12</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C9" s="10" t="str">
-        <f>Cancel!G12</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D9" s="10" t="str">
-        <f>Submit!N12</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=3_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>375</v>
-      </c>
-      <c r="B10" s="10" t="str">
-        <f>Start!J13</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=4_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C10" s="10" t="str">
-        <f>Cancel!G13</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D10" s="10" t="str">
-        <f>Submit!N13</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=4_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>376</v>
-      </c>
-      <c r="B11" s="10" t="str">
-        <f>Start!J14</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C11" s="10" t="str">
-        <f>Cancel!G14</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D11" s="10" t="str">
-        <f>Submit!N14</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=5_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>377</v>
-      </c>
-      <c r="B12" s="10" t="str">
-        <f>Start!J15</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C12" s="10" t="str">
-        <f>Cancel!G15</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D12" s="10" t="str">
-        <f>Submit!N15</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=6_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>378</v>
-      </c>
-      <c r="B13" s="10" t="str">
-        <f>Start!J16</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=7_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C13" s="10" t="str">
-        <f>Cancel!G16</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D13" s="10" t="str">
-        <f>Submit!N16</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=7_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>379</v>
-      </c>
-      <c r="B14" s="10" t="str">
-        <f>Start!J17</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C14" s="10" t="str">
-        <f>Cancel!G17</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D14" s="10" t="str">
-        <f>Submit!N17</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=8_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="B15" s="10" t="str">
-        <f>Start!J18</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C15" s="10" t="str">
-        <f>Cancel!G18</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D15" s="10" t="str">
-        <f>Submit!N18</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=9_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>381</v>
-      </c>
-      <c r="B16" s="10" t="str">
-        <f>Start!J19</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=10_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C16" s="10" t="str">
-        <f>Cancel!G19</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D16" s="10" t="str">
-        <f>Submit!N19</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=10_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>370</v>
-      </c>
-      <c r="B17" s="10" t="str">
-        <f>Start!J20</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=4_0xHdacb=5</v>
-      </c>
-      <c r="C17" s="10" t="str">
-        <f>Cancel!G20</f>
-        <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
-      </c>
-      <c r="D17" s="10" t="str">
-        <f>Submit!N20</f>
-        <v>0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>382</v>
-      </c>
-      <c r="B18" s="10" t="str">
         <f>Start!J21</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C18" s="10" t="str">
+      <c r="D6" s="10" t="str">
         <f>Cancel!G21</f>
         <v>0xNda19=0_0xMdaca=1_d0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="D18" s="10" t="str">
+      <c r="E6" s="10" t="str">
         <f>Submit!N21</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=11_d0xHdacb=5_0xHdacb=6</v>
       </c>
-      <c r="E18" s="10" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="F6" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="B19" s="10" t="str">
+      <c r="B7" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="C7" s="10" t="str">
         <f>Start!J22</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10" t="str">
+      <c r="D7" s="10"/>
+      <c r="E7" s="10" t="str">
         <f>Submit!N22</f>
         <v>0xNda19=0_0xMdaca=1S0xHdacd=11_d0xHdacb=5_0xHdacb=6Sd0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="F7" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
         <v>369</v>
       </c>
-      <c r="B20" s="10" t="str">
+      <c r="B8" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="C8" s="10" t="str">
         <f>Start!J23</f>
         <v>0xNda19=0_0xMdaca=1_0xHdacd=0_d0xHdacb=4_0xHdacb=5</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10" t="str">
+      <c r="D8" s="10"/>
+      <c r="E8" s="10" t="str">
         <f>Submit!N23</f>
         <v>0xNda19=0_0xMdaca=1S0xHdacd=11_d0xHdacb=5_0xHdacb=6Sd0xHdacb=12_0xHdacb=9</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>411</v>
-      </c>
-      <c r="B21" s="10" t="str">
+      <c r="F8" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>426</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>395</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="C14" s="10" t="str">
         <f>Start!J24</f>
         <v>0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10" t="str">
+      <c r="D14" s="10"/>
+      <c r="E14" s="10" t="str">
         <f>Submit!N24</f>
         <v>0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="B22" s="10" t="str">
+      <c r="B15" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="C15" s="10" t="str">
         <f>Start!J25</f>
         <v>0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10" t="str">
+      <c r="D15" s="10"/>
+      <c r="E15" s="10" t="str">
         <f>Submit!N25</f>
         <v>0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="F15" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
         <v>368</v>
       </c>
-      <c r="B23" s="10" t="str">
+      <c r="B16" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="C16" s="10" t="str">
         <f>Start!J26</f>
         <v>0xNda19=0_0xMdaca=0_0xHda24=1_d0xHcaff=19_0xHcaff=8</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10" t="str">
+      <c r="D16" s="10"/>
+      <c r="E16" s="10" t="str">
         <f>Submit!N26</f>
         <v>0xNda19=0_0xMdaca=0_d0xHda26=8_0xHda26=0</v>
       </c>
-      <c r="E23" s="10" t="s">
-        <v>387</v>
+      <c r="F16" s="10" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>
@@ -62046,7 +62023,7 @@
         <v>161</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -62058,25 +62035,25 @@
         <v>148</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>164</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="F4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="H4" s="23" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="I4" s="10" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>77</v>
@@ -62094,7 +62071,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F5" s="23">
         <v>4</v>
@@ -62127,7 +62104,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F6" s="23">
         <v>4</v>
@@ -62160,7 +62137,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F7" s="23">
         <v>4</v>
@@ -62193,7 +62170,7 @@
         <v>9</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F8" s="23">
         <v>4</v>
@@ -62226,7 +62203,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F9" s="23">
         <v>4</v>
@@ -62259,7 +62236,7 @@
         <v>1</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F10" s="23">
         <v>4</v>
@@ -62292,7 +62269,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F11" s="23">
         <v>4</v>
@@ -62325,7 +62302,7 @@
         <v>3</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F12" s="23">
         <v>4</v>
@@ -62358,7 +62335,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F13" s="23">
         <v>4</v>
@@ -62391,7 +62368,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F14" s="23">
         <v>4</v>
@@ -62424,7 +62401,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F15" s="23">
         <v>4</v>
@@ -62457,7 +62434,7 @@
         <v>7</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F16" s="23">
         <v>4</v>
@@ -62490,7 +62467,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F17" s="23">
         <v>4</v>
@@ -62523,7 +62500,7 @@
         <v>9</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F18" s="23">
         <v>4</v>
@@ -62556,7 +62533,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F19" s="23">
         <v>4</v>
@@ -62589,7 +62566,7 @@
         <v>11</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F20" s="23">
         <v>4</v>
@@ -62623,7 +62600,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F21" s="23">
         <v>4</v>
@@ -62657,7 +62634,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F22" s="23">
         <v>4</v>
@@ -62691,7 +62668,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="F23" s="23">
         <v>4</v>
@@ -62727,7 +62704,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="F24" s="23">
         <v>13</v>
@@ -62763,7 +62740,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="F25" s="23">
         <v>13</v>
@@ -62799,7 +62776,7 @@
         <v>1</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="F26" s="23">
         <v>13</v>

</xml_diff>